<commit_message>
Upload the project document
</commit_message>
<xml_diff>
--- a/documentation/BurndownChart/COMP3111_Project_GP19_BurndownChart.xlsx
+++ b/documentation/BurndownChart/COMP3111_Project_GP19_BurndownChart.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hkustconnect-my.sharepoint.com/personal/nslauaa_connect_ust_hk/Documents/2022-2023/22-23_SpringTerm/COMP3111/Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hkustconnect-my.sharepoint.com/personal/nslauaa_connect_ust_hk/Documents/2022-2023/22-23_SpringTerm/COMP3111/Project/GP19_Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="431" documentId="8_{F39DC93F-7446-49AE-A3B3-3247943C2370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07846D51-638C-4C84-B373-0E8AC9E2F4A1}"/>
+  <xr:revisionPtr revIDLastSave="560" documentId="8_{F39DC93F-7446-49AE-A3B3-3247943C2370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10004D7A-8A9E-42F3-BFC7-8EAEAEF7C9DD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{02C6DAF8-0742-46B5-ADA9-18D771A36031}"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="30936" windowHeight="17040" activeTab="1" xr2:uid="{02C6DAF8-0742-46B5-ADA9-18D771A36031}"/>
   </bookViews>
   <sheets>
-    <sheet name="FunA_LauNgaSze" sheetId="1" r:id="rId1"/>
-    <sheet name="FunB_CheungKwokWai" sheetId="2" r:id="rId2"/>
-    <sheet name="FunC_LeeChunYin" sheetId="3" r:id="rId3"/>
+    <sheet name="Overall" sheetId="4" r:id="rId1"/>
+    <sheet name="FunA_LauNgaSze" sheetId="1" r:id="rId2"/>
+    <sheet name="FunB_CheungKwokWai" sheetId="2" r:id="rId3"/>
+    <sheet name="FunC_LeeChunYin" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="27">
   <si>
     <t>Write JX documentation</t>
   </si>
@@ -105,12 +106,27 @@
   <si>
     <t>Task allocation (Function C)</t>
   </si>
+  <si>
+    <t>11/3/2023</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Dates</t>
+  </si>
+  <si>
+    <t>Planned Tasks</t>
+  </si>
+  <si>
+    <t>Remaining Tasks</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,8 +150,63 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,8 +231,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -184,38 +273,90 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -231,9 +372,62 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="6" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink 2" xfId="3" xr:uid="{9264F17D-9E4D-4B14-9397-237B86275171}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{CDDFEF34-7F6F-4D3C-919B-C8B386F45740}"/>
+    <cellStyle name="Normal 2 2" xfId="2" xr:uid="{2334DFFE-617B-49F3-B784-DACC74CB3389}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -249,6 +443,1212 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-HK" b="1">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Burn</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-HK" b="1" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>down chart (PPC1 calculator)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-HK" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Planned Tasks</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Overall!$B$2:$B$59</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="58"/>
+                <c:pt idx="0">
+                  <c:v>44996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45005</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45006</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45007</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45008</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45009</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45010</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45011</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>45012</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>45013</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>45014</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>45015</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45016</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>45017</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>45018</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>45019</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>45020</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>45021</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>45022</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>45023</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>45024</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45025</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>45026</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>45027</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>45028</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>45029</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>45030</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>45031</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>45032</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>45033</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>45034</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>45035</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>45036</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45037</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>45038</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>45039</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45040</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45041</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>45042</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>45043</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>45044</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>45045</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>45046</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>45047</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>45048</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>45049</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>45050</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>45051</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>45052</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>45053</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Overall!$C$2:$C$59</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="58"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="General">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="General">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="General">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="General">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="General">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="General">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="General">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="41" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="44" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="45" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="46" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="General">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="52" formatCode="General">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="53" formatCode="General">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="54" formatCode="General">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="55" formatCode="General">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="56" formatCode="General">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="57" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B1B1-43BF-8505-7489B1E4C2B2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Remaining Tasks</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Overall!$B$2:$B$59</c:f>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
+                <c:ptCount val="58"/>
+                <c:pt idx="0">
+                  <c:v>44996</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>44999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>45002</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>45003</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45004</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45005</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>45006</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>45007</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>45008</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>45009</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>45010</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>45011</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>45012</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>45013</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>45014</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>45015</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>45016</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>45017</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>45018</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>45019</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>45020</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>45021</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>45022</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>45023</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>45024</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45025</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>45026</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>45027</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>45028</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>45029</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>45030</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>45031</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>45032</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>45033</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>45034</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>45035</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>45036</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>45037</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>45038</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>45039</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45040</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45041</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>45042</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>45043</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>45044</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>45045</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>45046</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>45047</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>45048</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>45049</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>45050</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>45051</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>45052</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>45053</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Overall!$D$2:$D$59</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="58"/>
+                <c:pt idx="0">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="8" formatCode="General">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="15" formatCode="General">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="16" formatCode="General">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="17" formatCode="General">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="18" formatCode="General">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="19" formatCode="General">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="20" formatCode="General">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="21" formatCode="General">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="22" formatCode="General">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="23" formatCode="General">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="24" formatCode="General">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="25" formatCode="General">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="26" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="27" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="28" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="29" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="30" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="31" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="32" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="33" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="34" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="35" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="36" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="37" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="38" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="39" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="40" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="41" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="42" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="43" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="44" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="45" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="46" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="47" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="48" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="49" formatCode="General">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="50" formatCode="General">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="51" formatCode="General">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="52" formatCode="General">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="53" formatCode="General">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="54" formatCode="General">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="55" formatCode="General">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="56" formatCode="General">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="57" formatCode="General">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B1B1-43BF-8505-7489B1E4C2B2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="446992816"/>
+        <c:axId val="446993296"/>
+      </c:lineChart>
+      <c:dateAx>
+        <c:axId val="446992816"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-HK" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Working dates</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="446993296"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblOffset val="100"/>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
+      <c:valAx>
+        <c:axId val="446993296"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-HK" b="1">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Total</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-HK" b="1" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> remaining working days</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-HK" b="1">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="446992816"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -426,36 +1826,37 @@
             </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>FunA_LauNgaSze!$B$2:$G$2</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1/5/2023</c:v>
+                  <c:v>45047</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2/5/2023</c:v>
+                  <c:v>45048</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3/5/2023</c:v>
+                  <c:v>45049</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4/5/2023</c:v>
+                  <c:v>45050</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5/5/2023</c:v>
+                  <c:v>45051</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6/5/2023</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>45052</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
               <c:f>FunA_LauNgaSze!$B$8:$G$8</c:f>
               <c:numCache>
-                <c:formatCode>0</c:formatCode>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
                   <c:v>30</c:v>
@@ -499,7 +1900,7 @@
         <c:axId val="1317869135"/>
         <c:axId val="1317869615"/>
       </c:lineChart>
-      <c:catAx>
+      <c:dateAx>
         <c:axId val="1317869135"/>
         <c:scaling>
           <c:orientation val="minMax"/>
@@ -573,7 +1974,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="m/d/yyyy" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -613,10 +2014,9 @@
         <c:crossAx val="1317869615"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:baseTimeUnit val="days"/>
+      </c:dateAx>
       <c:valAx>
         <c:axId val="1317869615"/>
         <c:scaling>
@@ -710,7 +2110,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -797,7 +2197,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -967,7 +2367,7 @@
               <c:strCache>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1/5/2023</c:v>
+                  <c:v>11/3/2023</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>2/5/2023</c:v>
@@ -1312,7 +2712,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1935,8 +3335,48 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -2044,6 +3484,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -2054,6 +3499,11 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -2085,6 +3535,9 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3444,7 +4897,551 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>61545</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>67406</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>586154</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>164123</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA079D55-375F-D07C-092F-30207D8B54E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3485,7 +5482,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3526,7 +5523,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -3867,191 +5864,1064 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B06F9A14-E7D9-498B-B17F-56B2C5EED922}">
+  <dimension ref="A1:G59"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.21875" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="18">
+        <v>1</v>
+      </c>
+      <c r="B2" s="16">
+        <v>44996</v>
+      </c>
+      <c r="C2" s="19">
+        <v>15</v>
+      </c>
+      <c r="D2" s="21">
+        <v>15</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="18">
+        <v>2</v>
+      </c>
+      <c r="B3" s="16">
+        <v>44997</v>
+      </c>
+      <c r="C3" s="19">
+        <v>15</v>
+      </c>
+      <c r="D3" s="21">
+        <v>14</v>
+      </c>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="18">
+        <v>3</v>
+      </c>
+      <c r="B4" s="16">
+        <v>44998</v>
+      </c>
+      <c r="C4" s="20">
+        <v>14</v>
+      </c>
+      <c r="D4" s="21">
+        <v>14</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="18">
+        <v>4</v>
+      </c>
+      <c r="B5" s="16">
+        <v>44999</v>
+      </c>
+      <c r="C5" s="20">
+        <v>14</v>
+      </c>
+      <c r="D5" s="21">
+        <v>14</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="18">
+        <v>5</v>
+      </c>
+      <c r="B6" s="16">
+        <v>45000</v>
+      </c>
+      <c r="C6" s="20">
+        <v>14</v>
+      </c>
+      <c r="D6" s="21">
+        <v>14</v>
+      </c>
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="18">
+        <v>6</v>
+      </c>
+      <c r="B7" s="16">
+        <v>45001</v>
+      </c>
+      <c r="C7" s="20">
+        <v>14</v>
+      </c>
+      <c r="D7" s="21">
+        <v>14</v>
+      </c>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="18">
+        <v>7</v>
+      </c>
+      <c r="B8" s="16">
+        <v>45002</v>
+      </c>
+      <c r="C8" s="20">
+        <v>14</v>
+      </c>
+      <c r="D8" s="22">
+        <v>13</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="18">
+        <v>8</v>
+      </c>
+      <c r="B9" s="16">
+        <v>45003</v>
+      </c>
+      <c r="C9" s="20">
+        <v>13</v>
+      </c>
+      <c r="D9" s="22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="18">
+        <v>9</v>
+      </c>
+      <c r="B10" s="16">
+        <v>45004</v>
+      </c>
+      <c r="C10" s="20">
+        <v>13</v>
+      </c>
+      <c r="D10" s="22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="18">
+        <v>10</v>
+      </c>
+      <c r="B11" s="16">
+        <v>45005</v>
+      </c>
+      <c r="C11" s="20">
+        <v>13</v>
+      </c>
+      <c r="D11" s="22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="18">
+        <v>11</v>
+      </c>
+      <c r="B12" s="16">
+        <v>45006</v>
+      </c>
+      <c r="C12" s="20">
+        <v>13</v>
+      </c>
+      <c r="D12" s="22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="18">
+        <v>12</v>
+      </c>
+      <c r="B13" s="16">
+        <v>45007</v>
+      </c>
+      <c r="C13" s="20">
+        <v>11</v>
+      </c>
+      <c r="D13" s="22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="18">
+        <v>13</v>
+      </c>
+      <c r="B14" s="16">
+        <v>45008</v>
+      </c>
+      <c r="C14" s="20">
+        <v>11</v>
+      </c>
+      <c r="D14" s="22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="18">
+        <v>14</v>
+      </c>
+      <c r="B15" s="16">
+        <v>45009</v>
+      </c>
+      <c r="C15" s="20">
+        <v>11</v>
+      </c>
+      <c r="D15" s="22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="18">
+        <v>15</v>
+      </c>
+      <c r="B16" s="16">
+        <v>45010</v>
+      </c>
+      <c r="C16" s="20">
+        <v>11</v>
+      </c>
+      <c r="D16" s="22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="18">
+        <v>16</v>
+      </c>
+      <c r="B17" s="16">
+        <v>45011</v>
+      </c>
+      <c r="C17" s="20">
+        <v>10</v>
+      </c>
+      <c r="D17" s="22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="16">
+        <v>45012</v>
+      </c>
+      <c r="C18" s="20">
+        <v>10</v>
+      </c>
+      <c r="D18" s="22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="18">
+        <v>18</v>
+      </c>
+      <c r="B19" s="16">
+        <v>45013</v>
+      </c>
+      <c r="C19" s="20">
+        <v>10</v>
+      </c>
+      <c r="D19" s="22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="18">
+        <v>19</v>
+      </c>
+      <c r="B20" s="16">
+        <v>45014</v>
+      </c>
+      <c r="C20" s="20">
+        <v>10</v>
+      </c>
+      <c r="D20" s="22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="18">
+        <v>20</v>
+      </c>
+      <c r="B21" s="16">
+        <v>45015</v>
+      </c>
+      <c r="C21" s="20">
+        <v>10</v>
+      </c>
+      <c r="D21" s="22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="18">
+        <v>21</v>
+      </c>
+      <c r="B22" s="16">
+        <v>45016</v>
+      </c>
+      <c r="C22" s="20">
+        <v>10</v>
+      </c>
+      <c r="D22" s="22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23" s="18">
+        <v>22</v>
+      </c>
+      <c r="B23" s="16">
+        <v>45017</v>
+      </c>
+      <c r="C23" s="20">
+        <v>10</v>
+      </c>
+      <c r="D23" s="22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24" s="18">
+        <v>23</v>
+      </c>
+      <c r="B24" s="16">
+        <v>45018</v>
+      </c>
+      <c r="C24" s="20">
+        <v>10</v>
+      </c>
+      <c r="D24" s="22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25" s="18">
+        <v>24</v>
+      </c>
+      <c r="B25" s="16">
+        <v>45019</v>
+      </c>
+      <c r="C25" s="20">
+        <v>9</v>
+      </c>
+      <c r="D25" s="22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="18">
+        <v>25</v>
+      </c>
+      <c r="B26" s="16">
+        <v>45020</v>
+      </c>
+      <c r="C26" s="20">
+        <v>9</v>
+      </c>
+      <c r="D26" s="22">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27" s="18">
+        <v>26</v>
+      </c>
+      <c r="B27" s="16">
+        <v>45021</v>
+      </c>
+      <c r="C27" s="20">
+        <v>9</v>
+      </c>
+      <c r="D27" s="22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="18">
+        <v>27</v>
+      </c>
+      <c r="B28" s="16">
+        <v>45022</v>
+      </c>
+      <c r="C28" s="20">
+        <v>8</v>
+      </c>
+      <c r="D28" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="18">
+        <v>28</v>
+      </c>
+      <c r="B29" s="16">
+        <v>45023</v>
+      </c>
+      <c r="C29" s="20">
+        <v>7</v>
+      </c>
+      <c r="D29" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30" s="18">
+        <v>29</v>
+      </c>
+      <c r="B30" s="16">
+        <v>45024</v>
+      </c>
+      <c r="C30" s="20">
+        <v>7</v>
+      </c>
+      <c r="D30" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31" s="18">
+        <v>30</v>
+      </c>
+      <c r="B31" s="16">
+        <v>45025</v>
+      </c>
+      <c r="C31" s="20">
+        <v>7</v>
+      </c>
+      <c r="D31" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32" s="18">
+        <v>31</v>
+      </c>
+      <c r="B32" s="16">
+        <v>45026</v>
+      </c>
+      <c r="C32" s="20">
+        <v>7</v>
+      </c>
+      <c r="D32" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33" s="18">
+        <v>32</v>
+      </c>
+      <c r="B33" s="16">
+        <v>45027</v>
+      </c>
+      <c r="C33" s="20">
+        <v>7</v>
+      </c>
+      <c r="D33" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="18">
+        <v>33</v>
+      </c>
+      <c r="B34" s="16">
+        <v>45028</v>
+      </c>
+      <c r="C34" s="20">
+        <v>7</v>
+      </c>
+      <c r="D34" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35" s="18">
+        <v>34</v>
+      </c>
+      <c r="B35" s="16">
+        <v>45029</v>
+      </c>
+      <c r="C35" s="20">
+        <v>7</v>
+      </c>
+      <c r="D35" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36" s="18">
+        <v>35</v>
+      </c>
+      <c r="B36" s="16">
+        <v>45030</v>
+      </c>
+      <c r="C36" s="20">
+        <v>7</v>
+      </c>
+      <c r="D36" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="18">
+        <v>36</v>
+      </c>
+      <c r="B37" s="16">
+        <v>45031</v>
+      </c>
+      <c r="C37" s="20">
+        <v>7</v>
+      </c>
+      <c r="D37" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="18">
+        <v>37</v>
+      </c>
+      <c r="B38" s="16">
+        <v>45032</v>
+      </c>
+      <c r="C38" s="20">
+        <v>7</v>
+      </c>
+      <c r="D38" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="18">
+        <v>38</v>
+      </c>
+      <c r="B39" s="16">
+        <v>45033</v>
+      </c>
+      <c r="C39" s="20">
+        <v>7</v>
+      </c>
+      <c r="D39" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="18">
+        <v>39</v>
+      </c>
+      <c r="B40" s="16">
+        <v>45034</v>
+      </c>
+      <c r="C40" s="20">
+        <v>7</v>
+      </c>
+      <c r="D40" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="18">
+        <v>40</v>
+      </c>
+      <c r="B41" s="16">
+        <v>45035</v>
+      </c>
+      <c r="C41" s="20">
+        <v>7</v>
+      </c>
+      <c r="D41" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="18">
+        <v>41</v>
+      </c>
+      <c r="B42" s="16">
+        <v>45036</v>
+      </c>
+      <c r="C42" s="20">
+        <v>7</v>
+      </c>
+      <c r="D42" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="18">
+        <v>42</v>
+      </c>
+      <c r="B43" s="16">
+        <v>45037</v>
+      </c>
+      <c r="C43" s="20">
+        <v>7</v>
+      </c>
+      <c r="D43" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="18">
+        <v>43</v>
+      </c>
+      <c r="B44" s="16">
+        <v>45038</v>
+      </c>
+      <c r="C44" s="20">
+        <v>7</v>
+      </c>
+      <c r="D44" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45" s="18">
+        <v>44</v>
+      </c>
+      <c r="B45" s="16">
+        <v>45039</v>
+      </c>
+      <c r="C45" s="20">
+        <v>7</v>
+      </c>
+      <c r="D45" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46" s="18">
+        <v>45</v>
+      </c>
+      <c r="B46" s="16">
+        <v>45040</v>
+      </c>
+      <c r="C46" s="20">
+        <v>7</v>
+      </c>
+      <c r="D46" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47" s="18">
+        <v>46</v>
+      </c>
+      <c r="B47" s="16">
+        <v>45041</v>
+      </c>
+      <c r="C47" s="20">
+        <v>7</v>
+      </c>
+      <c r="D47" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48" s="18">
+        <v>47</v>
+      </c>
+      <c r="B48" s="16">
+        <v>45042</v>
+      </c>
+      <c r="C48" s="20">
+        <v>7</v>
+      </c>
+      <c r="D48" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="18">
+        <v>48</v>
+      </c>
+      <c r="B49" s="16">
+        <v>45043</v>
+      </c>
+      <c r="C49" s="20">
+        <v>7</v>
+      </c>
+      <c r="D49" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="18">
+        <v>49</v>
+      </c>
+      <c r="B50" s="16">
+        <v>45044</v>
+      </c>
+      <c r="C50" s="20">
+        <v>7</v>
+      </c>
+      <c r="D50" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51" s="18">
+        <v>50</v>
+      </c>
+      <c r="B51" s="16">
+        <v>45045</v>
+      </c>
+      <c r="C51" s="20">
+        <v>7</v>
+      </c>
+      <c r="D51" s="22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="18">
+        <v>51</v>
+      </c>
+      <c r="B52" s="16">
+        <v>45046</v>
+      </c>
+      <c r="C52" s="20">
+        <v>7</v>
+      </c>
+      <c r="D52" s="22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="18">
+        <v>52</v>
+      </c>
+      <c r="B53" s="16">
+        <v>45047</v>
+      </c>
+      <c r="C53" s="20">
+        <v>6</v>
+      </c>
+      <c r="D53" s="22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54" s="18">
+        <v>53</v>
+      </c>
+      <c r="B54" s="16">
+        <v>45048</v>
+      </c>
+      <c r="C54" s="20">
+        <v>4</v>
+      </c>
+      <c r="D54" s="22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="18">
+        <v>54</v>
+      </c>
+      <c r="B55" s="16">
+        <v>45049</v>
+      </c>
+      <c r="C55" s="20">
+        <v>3</v>
+      </c>
+      <c r="D55" s="22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56" s="18">
+        <v>55</v>
+      </c>
+      <c r="B56" s="16">
+        <v>45050</v>
+      </c>
+      <c r="C56" s="20">
+        <v>3</v>
+      </c>
+      <c r="D56" s="22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57" s="18">
+        <v>56</v>
+      </c>
+      <c r="B57" s="16">
+        <v>45051</v>
+      </c>
+      <c r="C57" s="20">
+        <v>3</v>
+      </c>
+      <c r="D57" s="22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58" s="18">
+        <v>57</v>
+      </c>
+      <c r="B58" s="16">
+        <v>45052</v>
+      </c>
+      <c r="C58" s="20">
+        <v>3</v>
+      </c>
+      <c r="D58" s="22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59" s="18">
+        <v>58</v>
+      </c>
+      <c r="B59" s="16">
+        <v>45053</v>
+      </c>
+      <c r="C59" s="20">
+        <v>0</v>
+      </c>
+      <c r="D59" s="22">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE85D098-4E56-4E6C-82C3-51890599B2F0}">
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="45.85546875" customWidth="1"/>
-    <col min="2" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.88671875" customWidth="1"/>
+    <col min="2" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:8" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="9" t="s">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+    </row>
+    <row r="2" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="24">
+        <v>45047</v>
+      </c>
+      <c r="C2" s="24">
+        <v>45048</v>
+      </c>
+      <c r="D2" s="24">
+        <v>45049</v>
+      </c>
+      <c r="E2" s="24">
+        <v>45050</v>
+      </c>
+      <c r="F2" s="24">
+        <v>45051</v>
+      </c>
+      <c r="G2" s="24">
+        <v>45052</v>
+      </c>
+      <c r="H2" s="1"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="26">
+        <v>6</v>
+      </c>
+      <c r="C3" s="26">
+        <v>3</v>
+      </c>
+      <c r="D3" s="26">
         <v>2</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="E3" s="26">
+        <v>0</v>
+      </c>
+      <c r="F3" s="26">
+        <v>0</v>
+      </c>
+      <c r="G3" s="26">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="26">
+        <v>6</v>
+      </c>
+      <c r="C4" s="26">
+        <v>4</v>
+      </c>
+      <c r="D4" s="26">
         <v>3</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="E4" s="26">
+        <v>1</v>
+      </c>
+      <c r="F4" s="26">
+        <v>1</v>
+      </c>
+      <c r="G4" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="26">
+        <v>6</v>
+      </c>
+      <c r="C5" s="26">
+        <v>6</v>
+      </c>
+      <c r="D5" s="26">
         <v>4</v>
       </c>
-      <c r="E2" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="14" t="s">
+      <c r="E5" s="26">
+        <v>2</v>
+      </c>
+      <c r="F5" s="26">
+        <v>0</v>
+      </c>
+      <c r="G5" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="26">
         <v>6</v>
       </c>
-      <c r="G2" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="11">
+      <c r="C6" s="26">
         <v>6</v>
       </c>
-      <c r="C3" s="11">
+      <c r="D6" s="26">
+        <v>6</v>
+      </c>
+      <c r="E6" s="26">
+        <v>4</v>
+      </c>
+      <c r="F6" s="26">
+        <v>2</v>
+      </c>
+      <c r="G6" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="26">
+        <v>6</v>
+      </c>
+      <c r="C7" s="26">
+        <v>6</v>
+      </c>
+      <c r="D7" s="26">
+        <v>6</v>
+      </c>
+      <c r="E7" s="26">
+        <v>4</v>
+      </c>
+      <c r="F7" s="26">
         <v>3</v>
       </c>
-      <c r="D3" s="11">
-        <v>2</v>
-      </c>
-      <c r="E3" s="11">
+      <c r="G7" s="26">
         <v>0</v>
       </c>
-      <c r="F3" s="11">
-        <v>0</v>
-      </c>
-      <c r="G3" s="11">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+    </row>
+    <row r="8" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="28">
+        <v>30</v>
+      </c>
+      <c r="C8" s="28">
+        <v>25</v>
+      </c>
+      <c r="D8" s="28">
+        <v>21</v>
+      </c>
+      <c r="E8" s="28">
         <v>11</v>
       </c>
-      <c r="B4" s="11">
+      <c r="F8" s="28">
         <v>6</v>
       </c>
-      <c r="C4" s="11">
-        <v>4</v>
-      </c>
-      <c r="D4" s="11">
-        <v>3</v>
-      </c>
-      <c r="E4" s="11">
-        <v>1</v>
-      </c>
-      <c r="F4" s="11">
-        <v>1</v>
-      </c>
-      <c r="G4" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B5" s="11">
-        <v>6</v>
-      </c>
-      <c r="C5" s="11">
-        <v>6</v>
-      </c>
-      <c r="D5" s="11">
-        <v>4</v>
-      </c>
-      <c r="E5" s="11">
-        <v>2</v>
-      </c>
-      <c r="F5" s="11">
-        <v>0</v>
-      </c>
-      <c r="G5" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="11">
-        <v>6</v>
-      </c>
-      <c r="C6" s="11">
-        <v>6</v>
-      </c>
-      <c r="D6" s="11">
-        <v>6</v>
-      </c>
-      <c r="E6" s="11">
-        <v>4</v>
-      </c>
-      <c r="F6" s="11">
-        <v>2</v>
-      </c>
-      <c r="G6" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="11">
-        <v>6</v>
-      </c>
-      <c r="C7" s="11">
-        <v>6</v>
-      </c>
-      <c r="D7" s="11">
-        <v>6</v>
-      </c>
-      <c r="E7" s="11">
-        <v>4</v>
-      </c>
-      <c r="F7" s="11">
-        <v>3</v>
-      </c>
-      <c r="G7" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="12">
-        <v>30</v>
-      </c>
-      <c r="C8" s="12">
-        <v>25</v>
-      </c>
-      <c r="D8" s="12">
-        <v>21</v>
-      </c>
-      <c r="E8" s="12">
-        <v>11</v>
-      </c>
-      <c r="F8" s="12">
-        <v>6</v>
-      </c>
-      <c r="G8" s="12">
+      <c r="G8" s="28">
         <v>0</v>
       </c>
     </row>
@@ -4065,55 +6935,56 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F1CEBCE-846D-489F-BA9B-6551F8AA0393}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="7" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" customWidth="1"/>
+    <col min="3" max="7" width="9.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="16" t="s">
+      <c r="B2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>16</v>
       </c>
@@ -4136,7 +7007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -4159,7 +7030,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -4182,7 +7053,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -4205,7 +7076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -4228,26 +7099,26 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>30</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>24</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>16</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>9</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <v>4</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>0</v>
       </c>
     </row>
@@ -4255,12 +7126,13 @@
   <mergeCells count="1">
     <mergeCell ref="A1:G1"/>
   </mergeCells>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FA47962-146F-43EA-82B5-E59A8A43283D}">
   <dimension ref="A1:L8"/>
   <sheetViews>
@@ -4268,71 +7140,71 @@
       <selection sqref="A1:L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:12" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="10">
         <v>45042</v>
       </c>
-      <c r="C2" s="17">
+      <c r="C2" s="10">
         <v>45043</v>
       </c>
-      <c r="D2" s="17">
+      <c r="D2" s="10">
         <v>45044</v>
       </c>
-      <c r="E2" s="17">
+      <c r="E2" s="10">
         <v>45045</v>
       </c>
-      <c r="F2" s="17">
+      <c r="F2" s="10">
         <v>45046</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="J2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="L2" s="7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -4370,7 +7242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -4408,7 +7280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -4446,7 +7318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -4484,7 +7356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>1</v>
       </c>
@@ -4522,7 +7394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>19</v>
       </c>
@@ -4541,22 +7413,22 @@
       <c r="F8" s="2">
         <v>15</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>10</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <v>8</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <v>4</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
         <v>2</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="5">
         <v>1</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="5">
         <v>0</v>
       </c>
     </row>

</xml_diff>